<commit_message>
feat: added charts and graphs under image folder
</commit_message>
<xml_diff>
--- a/analysis/edcr (validation)/out/top_f1/cobalt_shift_new_20_results.xlsx
+++ b/analysis/edcr (validation)/out/top_f1/cobalt_shift_new_20_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="33">
   <si>
     <t>Model</t>
   </si>
@@ -106,7 +106,10 @@
     <t>detection_correction</t>
   </si>
   <si>
-    <t>Best Precision, Best Recall, Best F1</t>
+    <t>Best Recall, Best F1</t>
+  </si>
+  <si>
+    <t>Best Precision</t>
   </si>
   <si>
     <t>Worst F1</t>
@@ -558,13 +561,13 @@
         <v>0.7285714285714286</v>
       </c>
       <c r="H2">
-        <v>0.8</v>
+        <v>0.8225806451612904</v>
       </c>
       <c r="I2">
-        <v>0.5</v>
+        <v>0.6538461538461539</v>
       </c>
       <c r="J2">
-        <v>0.6153846153846154</v>
+        <v>0.7285714285714286</v>
       </c>
       <c r="K2">
         <v>0.1547619047619048</v>
@@ -579,22 +582,22 @@
         <v>0.8</v>
       </c>
       <c r="O2">
-        <v>0.03333333333333333</v>
+        <v>0.010752688172043</v>
       </c>
       <c r="P2">
-        <v>0.2692307692307693</v>
+        <v>0.1153846153846154</v>
       </c>
       <c r="Q2">
-        <v>0.1846153846153846</v>
+        <v>0.0714285714285714</v>
       </c>
       <c r="R2">
-        <v>0.04166666666666666</v>
+        <v>0.01307189542483659</v>
       </c>
       <c r="S2">
-        <v>0.5384615384615385</v>
+        <v>0.1764705882352942</v>
       </c>
       <c r="T2">
-        <v>0.3</v>
+        <v>0.09803921568627445</v>
       </c>
       <c r="U2" t="s">
         <v>30</v>
@@ -623,13 +626,13 @@
         <v>0.7285714285714286</v>
       </c>
       <c r="H3">
-        <v>0.8</v>
+        <v>0.8225806451612904</v>
       </c>
       <c r="I3">
-        <v>0.5</v>
+        <v>0.6538461538461539</v>
       </c>
       <c r="J3">
-        <v>0.6153846153846154</v>
+        <v>0.7285714285714286</v>
       </c>
       <c r="K3">
         <v>0.1547619047619048</v>
@@ -644,22 +647,22 @@
         <v>0.8</v>
       </c>
       <c r="O3">
-        <v>0.03333333333333333</v>
+        <v>0.010752688172043</v>
       </c>
       <c r="P3">
-        <v>0.2692307692307693</v>
+        <v>0.1153846153846154</v>
       </c>
       <c r="Q3">
-        <v>0.1846153846153846</v>
+        <v>0.0714285714285714</v>
       </c>
       <c r="R3">
-        <v>0.04166666666666666</v>
+        <v>0.01307189542483659</v>
       </c>
       <c r="S3">
-        <v>0.5384615384615385</v>
+        <v>0.1764705882352942</v>
       </c>
       <c r="T3">
-        <v>0.3</v>
+        <v>0.09803921568627445</v>
       </c>
       <c r="U3" t="s">
         <v>30</v>
@@ -688,13 +691,13 @@
         <v>0.7285714285714286</v>
       </c>
       <c r="H4">
-        <v>0.8</v>
+        <v>0.8225806451612904</v>
       </c>
       <c r="I4">
-        <v>0.5</v>
+        <v>0.6538461538461539</v>
       </c>
       <c r="J4">
-        <v>0.6153846153846154</v>
+        <v>0.7285714285714286</v>
       </c>
       <c r="K4">
         <v>0.1547619047619048</v>
@@ -709,22 +712,22 @@
         <v>0.7285714285714286</v>
       </c>
       <c r="O4">
-        <v>0.02258064516129032</v>
+        <v>0</v>
       </c>
       <c r="P4">
-        <v>0.1538461538461539</v>
+        <v>0</v>
       </c>
       <c r="Q4">
-        <v>0.1131868131868132</v>
+        <v>0</v>
       </c>
       <c r="R4">
-        <v>0.02822580645161291</v>
+        <v>0</v>
       </c>
       <c r="S4">
-        <v>0.3076923076923077</v>
+        <v>0</v>
       </c>
       <c r="T4">
-        <v>0.1839285714285715</v>
+        <v>0</v>
       </c>
       <c r="U4" t="s">
         <v>30</v>
@@ -753,13 +756,13 @@
         <v>0.7285714285714286</v>
       </c>
       <c r="H5">
-        <v>0.8</v>
+        <v>0.8225806451612904</v>
       </c>
       <c r="I5">
-        <v>0.5</v>
+        <v>0.6538461538461539</v>
       </c>
       <c r="J5">
-        <v>0.6153846153846154</v>
+        <v>0.7285714285714286</v>
       </c>
       <c r="K5">
         <v>0.1547619047619048</v>
@@ -774,22 +777,22 @@
         <v>0.7285714285714286</v>
       </c>
       <c r="O5">
-        <v>0.02258064516129032</v>
+        <v>0</v>
       </c>
       <c r="P5">
-        <v>0.1538461538461539</v>
+        <v>0</v>
       </c>
       <c r="Q5">
-        <v>0.1131868131868132</v>
+        <v>0</v>
       </c>
       <c r="R5">
-        <v>0.02822580645161291</v>
+        <v>0</v>
       </c>
       <c r="S5">
-        <v>0.3076923076923077</v>
+        <v>0</v>
       </c>
       <c r="T5">
-        <v>0.1839285714285715</v>
+        <v>0</v>
       </c>
       <c r="U5" t="s">
         <v>30</v>
@@ -818,13 +821,13 @@
         <v>0.7285714285714286</v>
       </c>
       <c r="H6">
-        <v>0.8</v>
+        <v>0.8225806451612904</v>
       </c>
       <c r="I6">
-        <v>0.5</v>
+        <v>0.6538461538461539</v>
       </c>
       <c r="J6">
-        <v>0.6153846153846154</v>
+        <v>0.7285714285714286</v>
       </c>
       <c r="K6">
         <v>0.1547619047619048</v>
@@ -839,22 +842,22 @@
         <v>0.7285714285714286</v>
       </c>
       <c r="O6">
-        <v>0.02258064516129032</v>
+        <v>0</v>
       </c>
       <c r="P6">
-        <v>0.1538461538461539</v>
+        <v>0</v>
       </c>
       <c r="Q6">
-        <v>0.1131868131868132</v>
+        <v>0</v>
       </c>
       <c r="R6">
-        <v>0.02822580645161291</v>
+        <v>0</v>
       </c>
       <c r="S6">
-        <v>0.3076923076923077</v>
+        <v>0</v>
       </c>
       <c r="T6">
-        <v>0.1839285714285715</v>
+        <v>0</v>
       </c>
       <c r="U6" t="s">
         <v>30</v>
@@ -880,13 +883,13 @@
         <v>0.7285714285714286</v>
       </c>
       <c r="H7">
-        <v>0.8</v>
+        <v>0.8225806451612904</v>
       </c>
       <c r="I7">
-        <v>0.5</v>
+        <v>0.6538461538461539</v>
       </c>
       <c r="J7">
-        <v>0.6153846153846154</v>
+        <v>0.7285714285714286</v>
       </c>
       <c r="K7">
         <v>0.1547619047619048</v>
@@ -901,22 +904,22 @@
         <v>0.8250000000000001</v>
       </c>
       <c r="O7">
-        <v>0.004878048780487809</v>
+        <v>-0.01770259638080252</v>
       </c>
       <c r="P7">
-        <v>0.3461538461538461</v>
+        <v>0.1923076923076923</v>
       </c>
       <c r="Q7">
-        <v>0.2096153846153846</v>
+        <v>0.09642857142857142</v>
       </c>
       <c r="R7">
-        <v>0.006097560975609762</v>
+        <v>-0.02152080344332855</v>
       </c>
       <c r="S7">
-        <v>0.6923076923076923</v>
+        <v>0.2941176470588235</v>
       </c>
       <c r="T7">
-        <v>0.340625</v>
+        <v>0.1323529411764706</v>
       </c>
       <c r="U7" t="s">
         <v>30</v>
@@ -945,13 +948,13 @@
         <v>0.7285714285714286</v>
       </c>
       <c r="H8">
-        <v>0.8</v>
+        <v>0.8225806451612904</v>
       </c>
       <c r="I8">
-        <v>0.5</v>
+        <v>0.6538461538461539</v>
       </c>
       <c r="J8">
-        <v>0.6153846153846154</v>
+        <v>0.7285714285714286</v>
       </c>
       <c r="K8">
         <v>0.1547619047619048</v>
@@ -966,22 +969,22 @@
         <v>0.8250000000000001</v>
       </c>
       <c r="O8">
-        <v>0.004878048780487809</v>
+        <v>-0.01770259638080252</v>
       </c>
       <c r="P8">
-        <v>0.3461538461538461</v>
+        <v>0.1923076923076923</v>
       </c>
       <c r="Q8">
-        <v>0.2096153846153846</v>
+        <v>0.09642857142857142</v>
       </c>
       <c r="R8">
-        <v>0.006097560975609762</v>
+        <v>-0.02152080344332855</v>
       </c>
       <c r="S8">
-        <v>0.6923076923076923</v>
+        <v>0.2941176470588235</v>
       </c>
       <c r="T8">
-        <v>0.340625</v>
+        <v>0.1323529411764706</v>
       </c>
       <c r="U8" t="s">
         <v>30</v>
@@ -1010,13 +1013,13 @@
         <v>0.7285714285714286</v>
       </c>
       <c r="H9">
-        <v>0.8</v>
+        <v>0.8225806451612904</v>
       </c>
       <c r="I9">
-        <v>0.5</v>
+        <v>0.6538461538461539</v>
       </c>
       <c r="J9">
-        <v>0.6153846153846154</v>
+        <v>0.7285714285714286</v>
       </c>
       <c r="K9">
         <v>0.1547619047619048</v>
@@ -1031,22 +1034,22 @@
         <v>0.7285714285714286</v>
       </c>
       <c r="O9">
-        <v>0.02258064516129032</v>
+        <v>0</v>
       </c>
       <c r="P9">
-        <v>0.1538461538461539</v>
+        <v>0</v>
       </c>
       <c r="Q9">
-        <v>0.1131868131868132</v>
+        <v>0</v>
       </c>
       <c r="R9">
-        <v>0.02822580645161291</v>
+        <v>0</v>
       </c>
       <c r="S9">
-        <v>0.3076923076923077</v>
+        <v>0</v>
       </c>
       <c r="T9">
-        <v>0.1839285714285715</v>
+        <v>0</v>
       </c>
       <c r="U9" t="s">
         <v>30</v>
@@ -1075,13 +1078,13 @@
         <v>0.7285714285714286</v>
       </c>
       <c r="H10">
-        <v>0.8</v>
+        <v>0.8225806451612904</v>
       </c>
       <c r="I10">
-        <v>0.5</v>
+        <v>0.6538461538461539</v>
       </c>
       <c r="J10">
-        <v>0.6153846153846154</v>
+        <v>0.7285714285714286</v>
       </c>
       <c r="K10">
         <v>0.1547619047619048</v>
@@ -1096,22 +1099,22 @@
         <v>0.7285714285714286</v>
       </c>
       <c r="O10">
-        <v>0.02258064516129032</v>
+        <v>0</v>
       </c>
       <c r="P10">
-        <v>0.1538461538461539</v>
+        <v>0</v>
       </c>
       <c r="Q10">
-        <v>0.1131868131868132</v>
+        <v>0</v>
       </c>
       <c r="R10">
-        <v>0.02822580645161291</v>
+        <v>0</v>
       </c>
       <c r="S10">
-        <v>0.3076923076923077</v>
+        <v>0</v>
       </c>
       <c r="T10">
-        <v>0.1839285714285715</v>
+        <v>0</v>
       </c>
       <c r="U10" t="s">
         <v>30</v>
@@ -1140,13 +1143,13 @@
         <v>0.7285714285714286</v>
       </c>
       <c r="H11">
-        <v>0.8</v>
+        <v>0.8225806451612904</v>
       </c>
       <c r="I11">
-        <v>0.5</v>
+        <v>0.6538461538461539</v>
       </c>
       <c r="J11">
-        <v>0.6153846153846154</v>
+        <v>0.7285714285714286</v>
       </c>
       <c r="K11">
         <v>0.1547619047619048</v>
@@ -1161,22 +1164,22 @@
         <v>0.7285714285714286</v>
       </c>
       <c r="O11">
-        <v>0.02258064516129032</v>
+        <v>0</v>
       </c>
       <c r="P11">
-        <v>0.1538461538461539</v>
+        <v>0</v>
       </c>
       <c r="Q11">
-        <v>0.1131868131868132</v>
+        <v>0</v>
       </c>
       <c r="R11">
-        <v>0.02822580645161291</v>
+        <v>0</v>
       </c>
       <c r="S11">
-        <v>0.3076923076923077</v>
+        <v>0</v>
       </c>
       <c r="T11">
-        <v>0.1839285714285715</v>
+        <v>0</v>
       </c>
       <c r="U11" t="s">
         <v>30</v>
@@ -1202,13 +1205,13 @@
         <v>0.7285714285714286</v>
       </c>
       <c r="H12">
-        <v>0.8</v>
+        <v>0.8225806451612904</v>
       </c>
       <c r="I12">
-        <v>0.5</v>
+        <v>0.6538461538461539</v>
       </c>
       <c r="J12">
-        <v>0.6153846153846154</v>
+        <v>0.7285714285714286</v>
       </c>
       <c r="K12">
         <v>0.1547619047619048</v>
@@ -1223,22 +1226,22 @@
         <v>0.8</v>
       </c>
       <c r="O12">
-        <v>0.03333333333333333</v>
+        <v>0.010752688172043</v>
       </c>
       <c r="P12">
-        <v>0.2692307692307693</v>
+        <v>0.1153846153846154</v>
       </c>
       <c r="Q12">
-        <v>0.1846153846153846</v>
+        <v>0.0714285714285714</v>
       </c>
       <c r="R12">
-        <v>0.04166666666666666</v>
+        <v>0.01307189542483659</v>
       </c>
       <c r="S12">
-        <v>0.5384615384615385</v>
+        <v>0.1764705882352942</v>
       </c>
       <c r="T12">
-        <v>0.3</v>
+        <v>0.09803921568627445</v>
       </c>
       <c r="U12" t="s">
         <v>30</v>
@@ -1267,13 +1270,13 @@
         <v>0.7285714285714286</v>
       </c>
       <c r="H13">
-        <v>0.8</v>
+        <v>0.8225806451612904</v>
       </c>
       <c r="I13">
-        <v>0.5</v>
+        <v>0.6538461538461539</v>
       </c>
       <c r="J13">
-        <v>0.6153846153846154</v>
+        <v>0.7285714285714286</v>
       </c>
       <c r="K13">
         <v>0.1547619047619048</v>
@@ -1288,22 +1291,22 @@
         <v>0.8</v>
       </c>
       <c r="O13">
-        <v>0.03333333333333333</v>
+        <v>0.010752688172043</v>
       </c>
       <c r="P13">
-        <v>0.2692307692307693</v>
+        <v>0.1153846153846154</v>
       </c>
       <c r="Q13">
-        <v>0.1846153846153846</v>
+        <v>0.0714285714285714</v>
       </c>
       <c r="R13">
-        <v>0.04166666666666666</v>
+        <v>0.01307189542483659</v>
       </c>
       <c r="S13">
-        <v>0.5384615384615385</v>
+        <v>0.1764705882352942</v>
       </c>
       <c r="T13">
-        <v>0.3</v>
+        <v>0.09803921568627445</v>
       </c>
       <c r="U13" t="s">
         <v>30</v>
@@ -1332,13 +1335,13 @@
         <v>0.7285714285714286</v>
       </c>
       <c r="H14">
-        <v>0.8</v>
+        <v>0.8225806451612904</v>
       </c>
       <c r="I14">
-        <v>0.5</v>
+        <v>0.6538461538461539</v>
       </c>
       <c r="J14">
-        <v>0.6153846153846154</v>
+        <v>0.7285714285714286</v>
       </c>
       <c r="K14">
         <v>0.1547619047619048</v>
@@ -1353,22 +1356,22 @@
         <v>0.7285714285714286</v>
       </c>
       <c r="O14">
-        <v>0.02258064516129032</v>
+        <v>0</v>
       </c>
       <c r="P14">
-        <v>0.1538461538461539</v>
+        <v>0</v>
       </c>
       <c r="Q14">
-        <v>0.1131868131868132</v>
+        <v>0</v>
       </c>
       <c r="R14">
-        <v>0.02822580645161291</v>
+        <v>0</v>
       </c>
       <c r="S14">
-        <v>0.3076923076923077</v>
+        <v>0</v>
       </c>
       <c r="T14">
-        <v>0.1839285714285715</v>
+        <v>0</v>
       </c>
       <c r="U14" t="s">
         <v>30</v>
@@ -1397,13 +1400,13 @@
         <v>0.7285714285714286</v>
       </c>
       <c r="H15">
-        <v>0.8</v>
+        <v>0.8225806451612904</v>
       </c>
       <c r="I15">
-        <v>0.5</v>
+        <v>0.6538461538461539</v>
       </c>
       <c r="J15">
-        <v>0.6153846153846154</v>
+        <v>0.7285714285714286</v>
       </c>
       <c r="K15">
         <v>0.1547619047619048</v>
@@ -1418,22 +1421,22 @@
         <v>0.7285714285714286</v>
       </c>
       <c r="O15">
-        <v>0.02258064516129032</v>
+        <v>0</v>
       </c>
       <c r="P15">
-        <v>0.1538461538461539</v>
+        <v>0</v>
       </c>
       <c r="Q15">
-        <v>0.1131868131868132</v>
+        <v>0</v>
       </c>
       <c r="R15">
-        <v>0.02822580645161291</v>
+        <v>0</v>
       </c>
       <c r="S15">
-        <v>0.3076923076923077</v>
+        <v>0</v>
       </c>
       <c r="T15">
-        <v>0.1839285714285715</v>
+        <v>0</v>
       </c>
       <c r="U15" t="s">
         <v>30</v>
@@ -1462,13 +1465,13 @@
         <v>0.7285714285714286</v>
       </c>
       <c r="H16">
-        <v>0.8</v>
+        <v>0.8225806451612904</v>
       </c>
       <c r="I16">
-        <v>0.5</v>
+        <v>0.6538461538461539</v>
       </c>
       <c r="J16">
-        <v>0.6153846153846154</v>
+        <v>0.7285714285714286</v>
       </c>
       <c r="K16">
         <v>0.1547619047619048</v>
@@ -1483,22 +1486,22 @@
         <v>0.7285714285714286</v>
       </c>
       <c r="O16">
-        <v>0.02258064516129032</v>
+        <v>0</v>
       </c>
       <c r="P16">
-        <v>0.1538461538461539</v>
+        <v>0</v>
       </c>
       <c r="Q16">
-        <v>0.1131868131868132</v>
+        <v>0</v>
       </c>
       <c r="R16">
-        <v>0.02822580645161291</v>
+        <v>0</v>
       </c>
       <c r="S16">
-        <v>0.3076923076923077</v>
+        <v>0</v>
       </c>
       <c r="T16">
-        <v>0.1839285714285715</v>
+        <v>0</v>
       </c>
       <c r="U16" t="s">
         <v>30</v>
@@ -1524,13 +1527,13 @@
         <v>0.7285714285714286</v>
       </c>
       <c r="H17">
-        <v>0.8</v>
+        <v>0.8225806451612904</v>
       </c>
       <c r="I17">
-        <v>0.5</v>
+        <v>0.6538461538461539</v>
       </c>
       <c r="J17">
-        <v>0.6153846153846154</v>
+        <v>0.7285714285714286</v>
       </c>
       <c r="K17">
         <v>0.1547619047619048</v>
@@ -1545,22 +1548,22 @@
         <v>0.8250000000000001</v>
       </c>
       <c r="O17">
-        <v>0.004878048780487809</v>
+        <v>-0.01770259638080252</v>
       </c>
       <c r="P17">
-        <v>0.3461538461538461</v>
+        <v>0.1923076923076923</v>
       </c>
       <c r="Q17">
-        <v>0.2096153846153846</v>
+        <v>0.09642857142857142</v>
       </c>
       <c r="R17">
-        <v>0.006097560975609762</v>
+        <v>-0.02152080344332855</v>
       </c>
       <c r="S17">
-        <v>0.6923076923076923</v>
+        <v>0.2941176470588235</v>
       </c>
       <c r="T17">
-        <v>0.340625</v>
+        <v>0.1323529411764706</v>
       </c>
       <c r="U17" t="s">
         <v>30</v>
@@ -1589,13 +1592,13 @@
         <v>0.7285714285714286</v>
       </c>
       <c r="H18">
-        <v>0.8</v>
+        <v>0.8225806451612904</v>
       </c>
       <c r="I18">
-        <v>0.5</v>
+        <v>0.6538461538461539</v>
       </c>
       <c r="J18">
-        <v>0.6153846153846154</v>
+        <v>0.7285714285714286</v>
       </c>
       <c r="K18">
         <v>0.1547619047619048</v>
@@ -1610,22 +1613,22 @@
         <v>0.8250000000000001</v>
       </c>
       <c r="O18">
-        <v>0.004878048780487809</v>
+        <v>-0.01770259638080252</v>
       </c>
       <c r="P18">
-        <v>0.3461538461538461</v>
+        <v>0.1923076923076923</v>
       </c>
       <c r="Q18">
-        <v>0.2096153846153846</v>
+        <v>0.09642857142857142</v>
       </c>
       <c r="R18">
-        <v>0.006097560975609762</v>
+        <v>-0.02152080344332855</v>
       </c>
       <c r="S18">
-        <v>0.6923076923076923</v>
+        <v>0.2941176470588235</v>
       </c>
       <c r="T18">
-        <v>0.340625</v>
+        <v>0.1323529411764706</v>
       </c>
       <c r="U18" t="s">
         <v>30</v>
@@ -1654,13 +1657,13 @@
         <v>0.7285714285714286</v>
       </c>
       <c r="H19">
-        <v>0.8</v>
+        <v>0.8225806451612904</v>
       </c>
       <c r="I19">
-        <v>0.5</v>
+        <v>0.6538461538461539</v>
       </c>
       <c r="J19">
-        <v>0.6153846153846154</v>
+        <v>0.7285714285714286</v>
       </c>
       <c r="K19">
         <v>0.1547619047619048</v>
@@ -1675,22 +1678,22 @@
         <v>0.7285714285714286</v>
       </c>
       <c r="O19">
-        <v>0.02258064516129032</v>
+        <v>0</v>
       </c>
       <c r="P19">
-        <v>0.1538461538461539</v>
+        <v>0</v>
       </c>
       <c r="Q19">
-        <v>0.1131868131868132</v>
+        <v>0</v>
       </c>
       <c r="R19">
-        <v>0.02822580645161291</v>
+        <v>0</v>
       </c>
       <c r="S19">
-        <v>0.3076923076923077</v>
+        <v>0</v>
       </c>
       <c r="T19">
-        <v>0.1839285714285715</v>
+        <v>0</v>
       </c>
       <c r="U19" t="s">
         <v>30</v>
@@ -1719,13 +1722,13 @@
         <v>0.7285714285714286</v>
       </c>
       <c r="H20">
-        <v>0.8</v>
+        <v>0.8225806451612904</v>
       </c>
       <c r="I20">
-        <v>0.5</v>
+        <v>0.6538461538461539</v>
       </c>
       <c r="J20">
-        <v>0.6153846153846154</v>
+        <v>0.7285714285714286</v>
       </c>
       <c r="K20">
         <v>0.1547619047619048</v>
@@ -1740,22 +1743,22 @@
         <v>0.7285714285714286</v>
       </c>
       <c r="O20">
-        <v>0.02258064516129032</v>
+        <v>0</v>
       </c>
       <c r="P20">
-        <v>0.1538461538461539</v>
+        <v>0</v>
       </c>
       <c r="Q20">
-        <v>0.1131868131868132</v>
+        <v>0</v>
       </c>
       <c r="R20">
-        <v>0.02822580645161291</v>
+        <v>0</v>
       </c>
       <c r="S20">
-        <v>0.3076923076923077</v>
+        <v>0</v>
       </c>
       <c r="T20">
-        <v>0.1839285714285715</v>
+        <v>0</v>
       </c>
       <c r="U20" t="s">
         <v>30</v>
@@ -1784,13 +1787,13 @@
         <v>0.7285714285714286</v>
       </c>
       <c r="H21">
-        <v>0.8</v>
+        <v>0.8225806451612904</v>
       </c>
       <c r="I21">
-        <v>0.5</v>
+        <v>0.6538461538461539</v>
       </c>
       <c r="J21">
-        <v>0.6153846153846154</v>
+        <v>0.7285714285714286</v>
       </c>
       <c r="K21">
         <v>0.1547619047619048</v>
@@ -1805,22 +1808,22 @@
         <v>0.7285714285714286</v>
       </c>
       <c r="O21">
-        <v>0.02258064516129032</v>
+        <v>0</v>
       </c>
       <c r="P21">
-        <v>0.1538461538461539</v>
+        <v>0</v>
       </c>
       <c r="Q21">
-        <v>0.1131868131868132</v>
+        <v>0</v>
       </c>
       <c r="R21">
-        <v>0.02822580645161291</v>
+        <v>0</v>
       </c>
       <c r="S21">
-        <v>0.3076923076923077</v>
+        <v>0</v>
       </c>
       <c r="T21">
-        <v>0.1839285714285715</v>
+        <v>0</v>
       </c>
       <c r="U21" t="s">
         <v>30</v>
@@ -1846,13 +1849,13 @@
         <v>0.3191489361702128</v>
       </c>
       <c r="H22">
-        <v>1</v>
+        <v>0.9375</v>
       </c>
       <c r="I22">
-        <v>0.0625</v>
+        <v>0.1923076923076923</v>
       </c>
       <c r="J22">
-        <v>0.1176470588235294</v>
+        <v>0.3191489361702128</v>
       </c>
       <c r="K22">
         <v>0.1547619047619048</v>
@@ -1867,22 +1870,22 @@
         <v>0.3191489361702128</v>
       </c>
       <c r="O22">
-        <v>-0.0625</v>
+        <v>0</v>
       </c>
       <c r="P22">
-        <v>0.1298076923076923</v>
+        <v>2.775557561562891E-17</v>
       </c>
       <c r="Q22">
-        <v>0.2015018773466834</v>
+        <v>0</v>
       </c>
       <c r="R22">
-        <v>-0.0625</v>
+        <v>0</v>
       </c>
       <c r="S22">
-        <v>2.076923076923077</v>
+        <v>1.443289932012704E-16</v>
       </c>
       <c r="T22">
-        <v>1.712765957446809</v>
+        <v>0</v>
       </c>
       <c r="U22" t="s">
         <v>31</v>
@@ -1911,13 +1914,13 @@
         <v>0.3191489361702128</v>
       </c>
       <c r="H23">
-        <v>1</v>
+        <v>0.9375</v>
       </c>
       <c r="I23">
-        <v>0.0625</v>
+        <v>0.1923076923076923</v>
       </c>
       <c r="J23">
-        <v>0.1176470588235294</v>
+        <v>0.3191489361702128</v>
       </c>
       <c r="K23">
         <v>0.1547619047619048</v>
@@ -1932,22 +1935,22 @@
         <v>0.3191489361702128</v>
       </c>
       <c r="O23">
-        <v>-0.0625</v>
+        <v>0</v>
       </c>
       <c r="P23">
-        <v>0.1298076923076923</v>
+        <v>2.775557561562891E-17</v>
       </c>
       <c r="Q23">
-        <v>0.2015018773466834</v>
+        <v>0</v>
       </c>
       <c r="R23">
-        <v>-0.0625</v>
+        <v>0</v>
       </c>
       <c r="S23">
-        <v>2.076923076923077</v>
+        <v>1.443289932012704E-16</v>
       </c>
       <c r="T23">
-        <v>1.712765957446809</v>
+        <v>0</v>
       </c>
       <c r="U23" t="s">
         <v>31</v>
@@ -1976,13 +1979,13 @@
         <v>0.3191489361702128</v>
       </c>
       <c r="H24">
-        <v>1</v>
+        <v>0.9375</v>
       </c>
       <c r="I24">
-        <v>0.0625</v>
+        <v>0.1923076923076923</v>
       </c>
       <c r="J24">
-        <v>0.1176470588235294</v>
+        <v>0.3191489361702128</v>
       </c>
       <c r="K24">
         <v>0.1547619047619048</v>
@@ -1997,22 +2000,22 @@
         <v>0.3711340206185568</v>
       </c>
       <c r="O24">
-        <v>-0.05263157894736847</v>
+        <v>0.009868421052631526</v>
       </c>
       <c r="P24">
-        <v>0.1682692307692308</v>
+        <v>0.03846153846153849</v>
       </c>
       <c r="Q24">
-        <v>0.2534869617950274</v>
+        <v>0.05198508444834399</v>
       </c>
       <c r="R24">
-        <v>-0.05263157894736847</v>
+        <v>0.01052631578947363</v>
       </c>
       <c r="S24">
-        <v>2.692307692307693</v>
+        <v>0.2000000000000002</v>
       </c>
       <c r="T24">
-        <v>2.154639175257733</v>
+        <v>0.1628865979381445</v>
       </c>
       <c r="U24" t="s">
         <v>31</v>
@@ -2041,13 +2044,13 @@
         <v>0.3191489361702128</v>
       </c>
       <c r="H25">
-        <v>1</v>
+        <v>0.9375</v>
       </c>
       <c r="I25">
-        <v>0.0625</v>
+        <v>0.1923076923076923</v>
       </c>
       <c r="J25">
-        <v>0.1176470588235294</v>
+        <v>0.3191489361702128</v>
       </c>
       <c r="K25">
         <v>0.1547619047619048</v>
@@ -2062,22 +2065,22 @@
         <v>0.3711340206185568</v>
       </c>
       <c r="O25">
-        <v>-0.05263157894736847</v>
+        <v>0.009868421052631526</v>
       </c>
       <c r="P25">
-        <v>0.1682692307692308</v>
+        <v>0.03846153846153849</v>
       </c>
       <c r="Q25">
-        <v>0.2534869617950274</v>
+        <v>0.05198508444834399</v>
       </c>
       <c r="R25">
-        <v>-0.05263157894736847</v>
+        <v>0.01052631578947363</v>
       </c>
       <c r="S25">
-        <v>2.692307692307693</v>
+        <v>0.2000000000000002</v>
       </c>
       <c r="T25">
-        <v>2.154639175257733</v>
+        <v>0.1628865979381445</v>
       </c>
       <c r="U25" t="s">
         <v>31</v>
@@ -2106,13 +2109,13 @@
         <v>0.3191489361702128</v>
       </c>
       <c r="H26">
-        <v>1</v>
+        <v>0.9375</v>
       </c>
       <c r="I26">
-        <v>0.0625</v>
+        <v>0.1923076923076923</v>
       </c>
       <c r="J26">
-        <v>0.1176470588235294</v>
+        <v>0.3191489361702128</v>
       </c>
       <c r="K26">
         <v>0.1547619047619048</v>
@@ -2127,22 +2130,22 @@
         <v>0.3711340206185568</v>
       </c>
       <c r="O26">
-        <v>-0.05263157894736847</v>
+        <v>0.009868421052631526</v>
       </c>
       <c r="P26">
-        <v>0.1682692307692308</v>
+        <v>0.03846153846153849</v>
       </c>
       <c r="Q26">
-        <v>0.2534869617950274</v>
+        <v>0.05198508444834399</v>
       </c>
       <c r="R26">
-        <v>-0.05263157894736847</v>
+        <v>0.01052631578947363</v>
       </c>
       <c r="S26">
-        <v>2.692307692307693</v>
+        <v>0.2000000000000002</v>
       </c>
       <c r="T26">
-        <v>2.154639175257733</v>
+        <v>0.1628865979381445</v>
       </c>
       <c r="U26" t="s">
         <v>31</v>
@@ -2168,13 +2171,13 @@
         <v>0.3191489361702128</v>
       </c>
       <c r="H27">
-        <v>1</v>
+        <v>0.9375</v>
       </c>
       <c r="I27">
-        <v>0.0625</v>
+        <v>0.1923076923076923</v>
       </c>
       <c r="J27">
-        <v>0.1176470588235294</v>
+        <v>0.3191489361702128</v>
       </c>
       <c r="K27">
         <v>0.1547619047619048</v>
@@ -2189,22 +2192,22 @@
         <v>0.3191489361702128</v>
       </c>
       <c r="O27">
-        <v>-0.0625</v>
+        <v>0</v>
       </c>
       <c r="P27">
-        <v>0.1298076923076923</v>
+        <v>2.775557561562891E-17</v>
       </c>
       <c r="Q27">
-        <v>0.2015018773466834</v>
+        <v>0</v>
       </c>
       <c r="R27">
-        <v>-0.0625</v>
+        <v>0</v>
       </c>
       <c r="S27">
-        <v>2.076923076923077</v>
+        <v>1.443289932012704E-16</v>
       </c>
       <c r="T27">
-        <v>1.712765957446809</v>
+        <v>0</v>
       </c>
       <c r="U27" t="s">
         <v>31</v>
@@ -2233,13 +2236,13 @@
         <v>0.3191489361702128</v>
       </c>
       <c r="H28">
-        <v>1</v>
+        <v>0.9375</v>
       </c>
       <c r="I28">
-        <v>0.0625</v>
+        <v>0.1923076923076923</v>
       </c>
       <c r="J28">
-        <v>0.1176470588235294</v>
+        <v>0.3191489361702128</v>
       </c>
       <c r="K28">
         <v>0.1547619047619048</v>
@@ -2254,22 +2257,22 @@
         <v>0.3191489361702128</v>
       </c>
       <c r="O28">
-        <v>-0.0625</v>
+        <v>0</v>
       </c>
       <c r="P28">
-        <v>0.1298076923076923</v>
+        <v>2.775557561562891E-17</v>
       </c>
       <c r="Q28">
-        <v>0.2015018773466834</v>
+        <v>0</v>
       </c>
       <c r="R28">
-        <v>-0.0625</v>
+        <v>0</v>
       </c>
       <c r="S28">
-        <v>2.076923076923077</v>
+        <v>1.443289932012704E-16</v>
       </c>
       <c r="T28">
-        <v>1.712765957446809</v>
+        <v>0</v>
       </c>
       <c r="U28" t="s">
         <v>31</v>
@@ -2298,13 +2301,13 @@
         <v>0.3191489361702128</v>
       </c>
       <c r="H29">
-        <v>1</v>
+        <v>0.9375</v>
       </c>
       <c r="I29">
-        <v>0.0625</v>
+        <v>0.1923076923076923</v>
       </c>
       <c r="J29">
-        <v>0.1176470588235294</v>
+        <v>0.3191489361702128</v>
       </c>
       <c r="K29">
         <v>0.1547619047619048</v>
@@ -2319,22 +2322,22 @@
         <v>0.3191489361702128</v>
       </c>
       <c r="O29">
-        <v>-0.0625</v>
+        <v>0</v>
       </c>
       <c r="P29">
-        <v>0.1298076923076923</v>
+        <v>2.775557561562891E-17</v>
       </c>
       <c r="Q29">
-        <v>0.2015018773466834</v>
+        <v>0</v>
       </c>
       <c r="R29">
-        <v>-0.0625</v>
+        <v>0</v>
       </c>
       <c r="S29">
-        <v>2.076923076923077</v>
+        <v>1.443289932012704E-16</v>
       </c>
       <c r="T29">
-        <v>1.712765957446809</v>
+        <v>0</v>
       </c>
       <c r="U29" t="s">
         <v>31</v>
@@ -2363,13 +2366,13 @@
         <v>0.3191489361702128</v>
       </c>
       <c r="H30">
-        <v>1</v>
+        <v>0.9375</v>
       </c>
       <c r="I30">
-        <v>0.0625</v>
+        <v>0.1923076923076923</v>
       </c>
       <c r="J30">
-        <v>0.1176470588235294</v>
+        <v>0.3191489361702128</v>
       </c>
       <c r="K30">
         <v>0.1547619047619048</v>
@@ -2384,22 +2387,22 @@
         <v>0.3191489361702128</v>
       </c>
       <c r="O30">
-        <v>-0.0625</v>
+        <v>0</v>
       </c>
       <c r="P30">
-        <v>0.1298076923076923</v>
+        <v>2.775557561562891E-17</v>
       </c>
       <c r="Q30">
-        <v>0.2015018773466834</v>
+        <v>0</v>
       </c>
       <c r="R30">
-        <v>-0.0625</v>
+        <v>0</v>
       </c>
       <c r="S30">
-        <v>2.076923076923077</v>
+        <v>1.443289932012704E-16</v>
       </c>
       <c r="T30">
-        <v>1.712765957446809</v>
+        <v>0</v>
       </c>
       <c r="U30" t="s">
         <v>31</v>
@@ -2428,13 +2431,13 @@
         <v>0.3191489361702128</v>
       </c>
       <c r="H31">
-        <v>1</v>
+        <v>0.9375</v>
       </c>
       <c r="I31">
-        <v>0.0625</v>
+        <v>0.1923076923076923</v>
       </c>
       <c r="J31">
-        <v>0.1176470588235294</v>
+        <v>0.3191489361702128</v>
       </c>
       <c r="K31">
         <v>0.1547619047619048</v>
@@ -2449,22 +2452,22 @@
         <v>0.3191489361702128</v>
       </c>
       <c r="O31">
-        <v>-0.0625</v>
+        <v>0</v>
       </c>
       <c r="P31">
-        <v>0.1298076923076923</v>
+        <v>2.775557561562891E-17</v>
       </c>
       <c r="Q31">
-        <v>0.2015018773466834</v>
+        <v>0</v>
       </c>
       <c r="R31">
-        <v>-0.0625</v>
+        <v>0</v>
       </c>
       <c r="S31">
-        <v>2.076923076923077</v>
+        <v>1.443289932012704E-16</v>
       </c>
       <c r="T31">
-        <v>1.712765957446809</v>
+        <v>0</v>
       </c>
       <c r="U31" t="s">
         <v>31</v>
@@ -2490,13 +2493,13 @@
         <v>0.024390243902439</v>
       </c>
       <c r="H32">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="I32">
-        <v>0</v>
+        <v>0.0128205128205128</v>
       </c>
       <c r="J32">
-        <v>0</v>
+        <v>0.024390243902439</v>
       </c>
       <c r="K32">
         <v>0.1547619047619048</v>
@@ -2511,25 +2514,28 @@
         <v>0.7272727272727272</v>
       </c>
       <c r="O32">
-        <v>0.6530612244897959</v>
+        <v>0.4030612244897959</v>
       </c>
       <c r="P32">
-        <v>0.8205128205128205</v>
+        <v>0.8076923076923077</v>
       </c>
       <c r="Q32">
-        <v>0.7272727272727272</v>
+        <v>0.7028824833702881</v>
       </c>
       <c r="R32">
-        <v>0</v>
+        <v>1.612244897959183</v>
       </c>
       <c r="S32">
-        <v>0</v>
+        <v>63.00000000000011</v>
       </c>
       <c r="T32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20">
+        <v>28.81818181818184</v>
+      </c>
+      <c r="U32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21">
       <c r="A33" t="s">
         <v>23</v>
       </c>
@@ -2552,13 +2558,13 @@
         <v>0.024390243902439</v>
       </c>
       <c r="H33">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="I33">
-        <v>0</v>
+        <v>0.0128205128205128</v>
       </c>
       <c r="J33">
-        <v>0</v>
+        <v>0.024390243902439</v>
       </c>
       <c r="K33">
         <v>0.1547619047619048</v>
@@ -2573,25 +2579,28 @@
         <v>0.6764705882352942</v>
       </c>
       <c r="O33">
-        <v>0.5476190476190477</v>
+        <v>0.2976190476190477</v>
       </c>
       <c r="P33">
-        <v>0.8846153846153846</v>
+        <v>0.8717948717948718</v>
       </c>
       <c r="Q33">
-        <v>0.6764705882352942</v>
+        <v>0.6520803443328551</v>
       </c>
       <c r="R33">
-        <v>0</v>
+        <v>1.190476190476191</v>
       </c>
       <c r="S33">
-        <v>0</v>
+        <v>68.00000000000011</v>
       </c>
       <c r="T33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20">
+        <v>26.73529411764709</v>
+      </c>
+      <c r="U33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21">
       <c r="A34" t="s">
         <v>23</v>
       </c>
@@ -2614,13 +2623,13 @@
         <v>0.024390243902439</v>
       </c>
       <c r="H34">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="I34">
-        <v>0</v>
+        <v>0.0128205128205128</v>
       </c>
       <c r="J34">
-        <v>0</v>
+        <v>0.024390243902439</v>
       </c>
       <c r="K34">
         <v>0.1547619047619048</v>
@@ -2635,25 +2644,28 @@
         <v>0.6901408450704225</v>
       </c>
       <c r="O34">
-        <v>0.765625</v>
+        <v>0.515625</v>
       </c>
       <c r="P34">
-        <v>0.6282051282051282</v>
+        <v>0.6153846153846154</v>
       </c>
       <c r="Q34">
-        <v>0.6901408450704225</v>
+        <v>0.6657506011679835</v>
       </c>
       <c r="R34">
-        <v>0</v>
+        <v>2.0625</v>
       </c>
       <c r="S34">
-        <v>0</v>
+        <v>48.00000000000009</v>
       </c>
       <c r="T34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20">
+        <v>27.29577464788735</v>
+      </c>
+      <c r="U34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21">
       <c r="A35" t="s">
         <v>23</v>
       </c>
@@ -2676,13 +2688,13 @@
         <v>0.024390243902439</v>
       </c>
       <c r="H35">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="I35">
-        <v>0</v>
+        <v>0.0128205128205128</v>
       </c>
       <c r="J35">
-        <v>0</v>
+        <v>0.024390243902439</v>
       </c>
       <c r="K35">
         <v>0.1547619047619048</v>
@@ -2697,25 +2709,28 @@
         <v>0.6901408450704225</v>
       </c>
       <c r="O35">
-        <v>0.765625</v>
+        <v>0.515625</v>
       </c>
       <c r="P35">
-        <v>0.6282051282051282</v>
+        <v>0.6153846153846154</v>
       </c>
       <c r="Q35">
-        <v>0.6901408450704225</v>
+        <v>0.6657506011679835</v>
       </c>
       <c r="R35">
-        <v>0</v>
+        <v>2.0625</v>
       </c>
       <c r="S35">
-        <v>0</v>
+        <v>48.00000000000009</v>
       </c>
       <c r="T35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20">
+        <v>27.29577464788735</v>
+      </c>
+      <c r="U35" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21">
       <c r="A36" t="s">
         <v>23</v>
       </c>
@@ -2738,13 +2753,13 @@
         <v>0.024390243902439</v>
       </c>
       <c r="H36">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="I36">
-        <v>0</v>
+        <v>0.0128205128205128</v>
       </c>
       <c r="J36">
-        <v>0</v>
+        <v>0.024390243902439</v>
       </c>
       <c r="K36">
         <v>0.1547619047619048</v>
@@ -2759,25 +2774,28 @@
         <v>0.6901408450704225</v>
       </c>
       <c r="O36">
-        <v>0.765625</v>
+        <v>0.515625</v>
       </c>
       <c r="P36">
-        <v>0.6282051282051282</v>
+        <v>0.6153846153846154</v>
       </c>
       <c r="Q36">
-        <v>0.6901408450704225</v>
+        <v>0.6657506011679835</v>
       </c>
       <c r="R36">
-        <v>0</v>
+        <v>2.0625</v>
       </c>
       <c r="S36">
-        <v>0</v>
+        <v>48.00000000000009</v>
       </c>
       <c r="T36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20">
+        <v>27.29577464788735</v>
+      </c>
+      <c r="U36" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -2797,13 +2815,13 @@
         <v>0.024390243902439</v>
       </c>
       <c r="H37">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="I37">
-        <v>0</v>
+        <v>0.0128205128205128</v>
       </c>
       <c r="J37">
-        <v>0</v>
+        <v>0.024390243902439</v>
       </c>
       <c r="K37">
         <v>0.1547619047619048</v>
@@ -2818,25 +2836,28 @@
         <v>0.7239263803680981</v>
       </c>
       <c r="O37">
-        <v>0.6941176470588235</v>
+        <v>0.4441176470588235</v>
       </c>
       <c r="P37">
-        <v>0.7564102564102564</v>
+        <v>0.7435897435897436</v>
       </c>
       <c r="Q37">
-        <v>0.7239263803680981</v>
+        <v>0.699536136465659</v>
       </c>
       <c r="R37">
-        <v>0</v>
+        <v>1.776470588235294</v>
       </c>
       <c r="S37">
-        <v>0</v>
+        <v>58.0000000000001</v>
       </c>
       <c r="T37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20">
+        <v>28.68098159509205</v>
+      </c>
+      <c r="U37" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21">
       <c r="A38" t="s">
         <v>23</v>
       </c>
@@ -2859,13 +2880,13 @@
         <v>0.024390243902439</v>
       </c>
       <c r="H38">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="I38">
-        <v>0</v>
+        <v>0.0128205128205128</v>
       </c>
       <c r="J38">
-        <v>0</v>
+        <v>0.024390243902439</v>
       </c>
       <c r="K38">
         <v>0.1547619047619048</v>
@@ -2880,25 +2901,28 @@
         <v>0.04761904761904762</v>
       </c>
       <c r="O38">
+        <v>0.08333333333333331</v>
+      </c>
+      <c r="P38">
+        <v>0.01282051282051284</v>
+      </c>
+      <c r="Q38">
+        <v>0.02322880371660862</v>
+      </c>
+      <c r="R38">
         <v>0.3333333333333333</v>
       </c>
-      <c r="P38">
-        <v>0.02564102564102564</v>
-      </c>
-      <c r="Q38">
-        <v>0.04761904761904762</v>
-      </c>
-      <c r="R38">
-        <v>0</v>
-      </c>
       <c r="S38">
-        <v>0</v>
+        <v>1.000000000000003</v>
       </c>
       <c r="T38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20">
+        <v>0.9523809523809541</v>
+      </c>
+      <c r="U38" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21">
       <c r="A39" t="s">
         <v>23</v>
       </c>
@@ -2921,13 +2945,13 @@
         <v>0.024390243902439</v>
       </c>
       <c r="H39">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="I39">
-        <v>0</v>
+        <v>0.0128205128205128</v>
       </c>
       <c r="J39">
-        <v>0</v>
+        <v>0.024390243902439</v>
       </c>
       <c r="K39">
         <v>0.1547619047619048</v>
@@ -2942,25 +2966,28 @@
         <v>0.7239263803680981</v>
       </c>
       <c r="O39">
-        <v>0.6941176470588235</v>
+        <v>0.4441176470588235</v>
       </c>
       <c r="P39">
-        <v>0.7564102564102564</v>
+        <v>0.7435897435897436</v>
       </c>
       <c r="Q39">
-        <v>0.7239263803680981</v>
+        <v>0.699536136465659</v>
       </c>
       <c r="R39">
-        <v>0</v>
+        <v>1.776470588235294</v>
       </c>
       <c r="S39">
-        <v>0</v>
+        <v>58.0000000000001</v>
       </c>
       <c r="T39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20">
+        <v>28.68098159509205</v>
+      </c>
+      <c r="U39" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21">
       <c r="A40" t="s">
         <v>23</v>
       </c>
@@ -2983,13 +3010,13 @@
         <v>0.024390243902439</v>
       </c>
       <c r="H40">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="I40">
-        <v>0</v>
+        <v>0.0128205128205128</v>
       </c>
       <c r="J40">
-        <v>0</v>
+        <v>0.024390243902439</v>
       </c>
       <c r="K40">
         <v>0.1547619047619048</v>
@@ -3004,25 +3031,28 @@
         <v>0.7239263803680981</v>
       </c>
       <c r="O40">
-        <v>0.6941176470588235</v>
+        <v>0.4441176470588235</v>
       </c>
       <c r="P40">
-        <v>0.7564102564102564</v>
+        <v>0.7435897435897436</v>
       </c>
       <c r="Q40">
-        <v>0.7239263803680981</v>
+        <v>0.699536136465659</v>
       </c>
       <c r="R40">
-        <v>0</v>
+        <v>1.776470588235294</v>
       </c>
       <c r="S40">
-        <v>0</v>
+        <v>58.0000000000001</v>
       </c>
       <c r="T40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20">
+        <v>28.68098159509205</v>
+      </c>
+      <c r="U40" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21">
       <c r="A41" t="s">
         <v>23</v>
       </c>
@@ -3045,13 +3075,13 @@
         <v>0.024390243902439</v>
       </c>
       <c r="H41">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="I41">
-        <v>0</v>
+        <v>0.0128205128205128</v>
       </c>
       <c r="J41">
-        <v>0</v>
+        <v>0.024390243902439</v>
       </c>
       <c r="K41">
         <v>0.1547619047619048</v>
@@ -3066,22 +3096,25 @@
         <v>0.7239263803680981</v>
       </c>
       <c r="O41">
-        <v>0.6941176470588235</v>
+        <v>0.4441176470588235</v>
       </c>
       <c r="P41">
-        <v>0.7564102564102564</v>
+        <v>0.7435897435897436</v>
       </c>
       <c r="Q41">
-        <v>0.7239263803680981</v>
+        <v>0.699536136465659</v>
       </c>
       <c r="R41">
-        <v>0</v>
+        <v>1.776470588235294</v>
       </c>
       <c r="S41">
-        <v>0</v>
+        <v>58.0000000000001</v>
       </c>
       <c r="T41">
-        <v>0</v>
+        <v>28.68098159509205</v>
+      </c>
+      <c r="U41" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>